<commit_message>
Added method what change columns names to original version with with spaces instead of underscore. All files checked by PYLINT and corrected
</commit_message>
<xml_diff>
--- a/deliveries_adding_OOP/data/processed_orders.xlsx
+++ b/deliveries_adding_OOP/data/processed_orders.xlsx
@@ -450,22 +450,22 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Purchase_order_number</t>
+          <t>Purchase order number</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Order_date</t>
+          <t>Order date</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Supplier_PO_number</t>
+          <t>Supplier PO number</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Order_confirmation_date</t>
+          <t>Order confirmation date</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -475,32 +475,32 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Customer_company</t>
+          <t>Customer company</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>SKU_NO</t>
+          <t>SKU NO</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Ordered_(kg)</t>
+          <t>Ordered (kg)</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Delivered_(kg)</t>
+          <t>Delivered (kg)</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>Current_delivery_date</t>
+          <t>Current delivery date</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Original_confirmed_quantity_(kg)</t>
+          <t>Original confirmed quantity (kg)</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
@@ -510,7 +510,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Original_confirmed_delivery_date</t>
+          <t>Original confirmed delivery date</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -520,32 +520,32 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Executed_delivery_date</t>
+          <t>Executed delivery date</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>Required_delivery_date_OTIF1</t>
+          <t>Required delivery date OTIF1</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>Required_quantity_OTIF1</t>
+          <t>Required quantity OTIF1</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>Delivery_not_on_time_reasons</t>
+          <t>Delivery not on time reasons</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Delivery_not_in_full_reasons</t>
+          <t>Delivery not in full reasons</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Delivery_documentation</t>
+          <t>Delivery documentation</t>
         </is>
       </c>
     </row>

</xml_diff>